<commit_message>
First version pie charts
See folder 10_Hierarchy. Also updated 09_pDC_expr to test for genes that upregulated in pre-malignant pDCs.
</commit_message>
<xml_diff>
--- a/04_XV-seq/XV-seq_overview.xlsx
+++ b/04_XV-seq/XV-seq_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/Github/4_XV-seq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/scBPDCN-analysis/04_XV-seq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C648CEA0-8A0A-0C4A-8FE1-6C0BEE33FF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742AC00B-A150-F748-AE50-EA090551ED77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="740" windowWidth="28660" windowHeight="24100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XV-seq_overview" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="242">
   <si>
     <t>Sample</t>
   </si>
@@ -746,6 +746,18 @@
   </si>
   <si>
     <t>Pt1Rem/SETX.10691/Patient1Rem_SETX.10691_summTable.txt</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>UV-associated (C&gt;T)</t>
+  </si>
+  <si>
+    <t>UV-associated (TC&gt;TT or CC&gt;TT)</t>
   </si>
 </sst>
 </file>
@@ -914,7 +926,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1100,6 +1112,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1279,7 +1297,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1350,6 +1368,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1746,11 +1768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7:L11"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1758,19 +1780,19 @@
     <col min="1" max="1" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18" style="5" customWidth="1"/>
-    <col min="10" max="10" width="85.83203125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16" style="32" customWidth="1"/>
-    <col min="12" max="12" width="61.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="5"/>
+    <col min="4" max="6" width="14.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="69.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="18" style="5" customWidth="1"/>
+    <col min="12" max="12" width="85.83203125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="16" style="32" customWidth="1"/>
+    <col min="14" max="14" width="61.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -1784,31 +1806,37 @@
         <v>227</v>
       </c>
       <c r="E1" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="H1" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1821,30 +1849,32 @@
       <c r="D2" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="4">
         <v>1.01091791346542</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="K2" s="25">
+      <c r="M2" s="25">
         <v>6415</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -1857,30 +1887,32 @@
       <c r="D3" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="4">
         <v>0.242620299231702</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="L3" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="K3" s="25">
+      <c r="M3" s="25">
         <v>2555</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -1893,32 +1925,36 @@
       <c r="D4" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="36"/>
+      <c r="G4" s="4">
         <v>2.9518803073190401</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="L4" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="K4" s="25">
+      <c r="M4" s="25">
         <v>225</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -1931,32 +1967,36 @@
       <c r="D5" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="4">
         <v>6.0250707642539396</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="L5" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="K5" s="26">
+      <c r="M5" s="26">
         <v>324</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
@@ -1969,32 +2009,36 @@
       <c r="D6" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="9">
         <v>4.5693489688637197</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="L6" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="K6" s="27">
+      <c r="M6" s="27">
         <v>120</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="N6" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>232</v>
       </c>
@@ -2007,30 +2051,32 @@
       <c r="D7" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="4">
         <v>1.0861132660977499</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>232</v>
       </c>
@@ -2043,30 +2089,32 @@
       <c r="D8" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="4">
         <v>0.28122575640031</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K8" s="29" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>232</v>
       </c>
@@ -2079,32 +2127,36 @@
       <c r="D9" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="36"/>
+      <c r="G9" s="4">
         <v>2.4825446082234199</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K9" s="29" t="s">
+      <c r="J9" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>232</v>
       </c>
@@ -2117,32 +2169,36 @@
       <c r="D10" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="36"/>
+      <c r="G10" s="4">
         <v>6.5554693560899899</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K10" s="29" t="s">
+      <c r="J10" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>232</v>
       </c>
@@ -2155,32 +2211,36 @@
       <c r="D11" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="9">
         <v>4.4511249030256002</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="K11" s="30" t="s">
+      <c r="J11" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>139</v>
       </c>
       <c r="L11" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="M11" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N11" s="8" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>56</v>
       </c>
@@ -2193,30 +2253,32 @@
       <c r="D12" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="4">
         <v>4.2702050663449898</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="20" t="s">
+      <c r="J12" s="3"/>
+      <c r="K12" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="L12" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="K12" s="25">
+      <c r="M12" s="25">
         <v>8449</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -2229,30 +2291,32 @@
       <c r="D13" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="4">
         <v>5.4764776839565696</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="20" t="s">
+      <c r="J13" s="3"/>
+      <c r="K13" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="L13" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="K13" s="25">
+      <c r="M13" s="25">
         <v>5109</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
         <v>56</v>
       </c>
@@ -2265,30 +2329,32 @@
       <c r="D14" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="9">
         <v>5.9831121833534304</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="8"/>
+      <c r="K14" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="L14" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="K14" s="27">
+      <c r="M14" s="27">
         <v>942</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="N14" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
@@ -2301,32 +2367,34 @@
       <c r="D15" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="4">
         <v>9.8609904430929607</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="J15" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="K15" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="L15" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="31">
+      <c r="M15" s="31">
         <v>5002</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -2339,32 +2407,34 @@
       <c r="D16" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="4">
         <v>3.8444830582102498</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="K16" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="K16" s="26">
+      <c r="M16" s="26">
         <v>4701</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
@@ -2377,32 +2447,34 @@
       <c r="D17" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="9">
         <v>1.62901824500434</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="K17" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="L17" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="K17" s="27">
+      <c r="M17" s="27">
         <v>11002</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="N17" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2415,32 +2487,36 @@
       <c r="D18" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="11">
         <v>1.22699386503067</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="K18" s="29">
+      <c r="M18" s="29">
         <v>6953</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -2453,32 +2529,36 @@
       <c r="D19" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="11">
         <v>1.0686720759944499</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K19" s="29">
+      <c r="M19" s="29">
         <v>6215</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
@@ -2491,32 +2571,34 @@
       <c r="D20" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="11">
         <v>1.1379378586978</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K20" s="29">
+      <c r="M20" s="29">
         <v>5667</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="N20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
@@ -2529,32 +2611,34 @@
       <c r="D21" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="11">
         <v>1.88007124480506</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K21" s="29">
+      <c r="M21" s="29">
         <v>5189</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
@@ -2567,32 +2651,36 @@
       <c r="D22" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="F22" s="38"/>
+      <c r="G22" s="11">
         <v>27.646942410449199</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K22" s="32">
+      <c r="M22" s="32">
         <v>6681</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="N22" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
@@ -2605,29 +2693,31 @@
       <c r="D23" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="11">
         <v>0.41559469622006701</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="K23" s="32">
+      <c r="M23" s="32">
         <v>2760</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="N23" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>37</v>
       </c>
@@ -2640,32 +2730,34 @@
       <c r="D24" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="11">
         <v>9.8357411438749196</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="I24" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K24" s="32">
+      <c r="M24" s="32">
         <v>2622</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="N24" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
@@ -2678,32 +2770,34 @@
       <c r="D25" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="11">
         <v>0.24737779536908699</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="I25" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="K25" s="32">
+      <c r="M25" s="32">
         <v>1515</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="N25" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
@@ -2716,32 +2810,36 @@
       <c r="D26" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F26" s="39"/>
+      <c r="G26" s="11">
         <v>6.1844448842271902</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="I26" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="K26" s="32">
+      <c r="M26" s="32">
         <v>1454</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="N26" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
@@ -2754,32 +2852,36 @@
       <c r="D27" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F27" s="39"/>
+      <c r="G27" s="11">
         <v>1.20720364140114</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="I27" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="K27" s="32">
+      <c r="M27" s="32">
         <v>2090</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="N27" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
         <v>37</v>
       </c>
@@ -2792,32 +2894,36 @@
       <c r="D28" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F28" s="39"/>
+      <c r="G28" s="11">
         <v>13.2000791608945</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="I28" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="K28" s="32">
+      <c r="M28" s="32">
         <v>1816</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="N28" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>37</v>
       </c>
@@ -2829,15 +2935,17 @@
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="16" t="s">
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>37</v>
       </c>
@@ -2849,15 +2957,17 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="16"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="16" t="s">
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>37</v>
       </c>
@@ -2869,15 +2979,17 @@
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
       <c r="J31" s="18"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="18" t="s">
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>37</v>
       </c>
@@ -2889,15 +3001,17 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
       <c r="J32" s="18"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="18" t="s">
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2910,32 +3024,34 @@
       <c r="D33" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="4">
         <v>35.751038986740497</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="I33" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="K33" s="29">
+      <c r="M33" s="29">
         <v>350</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:14" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -2948,32 +3064,34 @@
       <c r="D34" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="4">
         <v>98.990698594894099</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="I34" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="J34" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="K34" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="L34" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="K34" s="7">
+      <c r="M34" s="7">
         <v>421</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="N34" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>37</v>
       </c>
@@ -2986,32 +3104,34 @@
       <c r="D35" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="4">
         <v>4.8288145656045902</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="I35" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="J35" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="K35" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="L35" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="K35" s="7">
+      <c r="M35" s="7">
         <v>3296</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="N35" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8" t="s">
         <v>37</v>
       </c>
@@ -3024,32 +3144,34 @@
       <c r="D36" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="9">
         <v>0.77181872155155296</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="J36" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="K36" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="L36" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="K36" s="10">
+      <c r="M36" s="10">
         <v>1824</v>
       </c>
-      <c r="L36" s="8" t="s">
+      <c r="N36" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
@@ -3062,32 +3184,36 @@
       <c r="D37" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F37" s="36"/>
+      <c r="G37" s="4">
         <v>2.6940517471325598</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J37" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K37" s="29" t="s">
+      <c r="K37" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M37" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N37" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>23</v>
       </c>
@@ -3100,32 +3226,36 @@
       <c r="D38" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="4">
         <v>3.3208855694851902</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J38" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K38" s="29" t="s">
+      <c r="K38" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L38" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M38" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N38" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>23</v>
       </c>
@@ -3138,32 +3268,34 @@
       <c r="D39" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="4">
         <v>3.0808215524139699</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="I39" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J39" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K39" s="29" t="s">
+      <c r="K39" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L39" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M39" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N39" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>23</v>
       </c>
@@ -3176,32 +3308,34 @@
       <c r="D40" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="4">
         <v>5.1347025873566201</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="I40" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J40" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K40" s="29" t="s">
+      <c r="K40" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L40" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M40" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N40" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>23</v>
       </c>
@@ -3214,32 +3348,36 @@
       <c r="D41" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" s="38"/>
+      <c r="G41" s="4">
         <v>29.6345692184582</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="H41" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="I41" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J41" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K41" s="29" t="s">
+      <c r="K41" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N41" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
         <v>23</v>
       </c>
@@ -3252,30 +3390,32 @@
       <c r="D42" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="4">
         <v>0.89357161909842597</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K42" s="29" t="s">
+      <c r="J42" s="3"/>
+      <c r="K42" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L42" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M42" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N42" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
         <v>23</v>
       </c>
@@ -3288,32 +3428,34 @@
       <c r="D43" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="4">
         <v>10.282742064550501</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="I43" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J43" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K43" s="29" t="s">
+      <c r="K43" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L43" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M43" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N43" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>23</v>
       </c>
@@ -3326,32 +3468,34 @@
       <c r="D44" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="4">
         <v>0.25340090690850797</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="I44" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J44" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K44" s="29" t="s">
+      <c r="K44" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L44" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M44" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N44" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>23</v>
       </c>
@@ -3364,32 +3508,36 @@
       <c r="D45" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F45" s="39"/>
+      <c r="G45" s="4">
         <v>20.085356094958598</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="I45" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J45" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K45" s="29" t="s">
+      <c r="K45" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M45" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N45" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>23</v>
       </c>
@@ -3402,32 +3550,36 @@
       <c r="D46" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F46" s="39"/>
+      <c r="G46" s="4">
         <v>2.8007468658308801</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="I46" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K46" s="29" t="s">
+      <c r="K46" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L46" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M46" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N46" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>23</v>
       </c>
@@ -3440,32 +3592,36 @@
       <c r="D47" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F47" s="39"/>
+      <c r="G47" s="4">
         <v>28.540944251800401</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="I47" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J47" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K47" s="29" t="s">
+      <c r="K47" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L47" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M47" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N47" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A48" s="18" t="s">
         <v>23</v>
       </c>
@@ -3473,19 +3629,21 @@
       <c r="C48" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="19"/>
       <c r="J48" s="18"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="18" t="s">
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="34"/>
+      <c r="N48" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A49" s="18" t="s">
         <v>23</v>
       </c>
@@ -3493,19 +3651,21 @@
       <c r="C49" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="19"/>
       <c r="J49" s="18"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="18" t="s">
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A50" s="18" t="s">
         <v>23</v>
       </c>
@@ -3517,15 +3677,17 @@
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
       <c r="J50" s="18"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="18" t="s">
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A51" s="18" t="s">
         <v>23</v>
       </c>
@@ -3537,15 +3699,17 @@
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
       <c r="J51" s="18"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="18" t="s">
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A52" s="8" t="s">
         <v>23</v>
       </c>
@@ -3558,32 +3722,34 @@
       <c r="D52" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="9">
         <v>37.623366230994897</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="H52" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="I52" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H52" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="J52" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="K52" s="30" t="s">
+      <c r="K52" s="8" t="s">
         <v>139</v>
       </c>
       <c r="L52" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="M52" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N52" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -3596,30 +3762,32 @@
       <c r="D53" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="4">
         <v>0.39347129116875501</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="H53" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="I53" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6" t="s">
+      <c r="J53" s="6"/>
+      <c r="K53" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="J53" s="6" t="s">
+      <c r="L53" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="K53" s="6">
+      <c r="M53" s="6">
         <v>4684</v>
       </c>
-      <c r="L53" s="3" t="s">
+      <c r="N53" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -3632,32 +3800,34 @@
       <c r="D54" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="4">
         <v>8.7438064704167803E-2</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="H54" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="J54" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="I54" s="6" t="s">
+      <c r="K54" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="J54" s="6" t="s">
+      <c r="L54" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="K54" s="6" t="s">
+      <c r="M54" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="L54" s="3" t="s">
+      <c r="N54" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -3670,32 +3840,34 @@
       <c r="D55" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="4">
         <v>1.50102011075488</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="I55" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="J55" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="I55" s="6" t="s">
+      <c r="K55" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="J55" s="6" t="s">
+      <c r="L55" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="K55" s="6">
+      <c r="M55" s="6">
         <v>527</v>
       </c>
-      <c r="L55" s="3" t="s">
+      <c r="N55" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
         <v>57</v>
       </c>
@@ -3708,32 +3880,34 @@
       <c r="D56" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="9">
         <v>2.7980180705333701</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="H56" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="I56" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="J56" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="I56" s="10" t="s">
+      <c r="K56" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="J56" s="10" t="s">
+      <c r="L56" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="K56" s="10">
+      <c r="M56" s="10">
         <v>2572</v>
       </c>
-      <c r="L56" s="8" t="s">
+      <c r="N56" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -3746,30 +3920,32 @@
       <c r="D57" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="4">
         <v>22.822201317027201</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="H57" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="I57" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="J57" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="K57" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="L57" s="3" t="s">
+      <c r="J57" s="3"/>
+      <c r="K57" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="M57" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="N57" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>58</v>
       </c>
@@ -3782,32 +3958,34 @@
       <c r="D58" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="4">
         <v>11.0253998118532</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="H58" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="I58" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J58" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K58" s="29" t="s">
+      <c r="K58" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L58" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M58" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N58" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
@@ -3820,32 +3998,34 @@
       <c r="D59" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="4">
         <v>8.5042333019755407</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="I59" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H59" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="J59" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K59" s="29" t="s">
+      <c r="K59" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L59" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M59" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N59" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60" s="8" t="s">
         <v>58</v>
       </c>
@@ -3858,32 +4038,34 @@
       <c r="D60" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="9">
         <v>8.4101599247412899</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="H60" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="I60" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H60" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="J60" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="K60" s="30" t="s">
+      <c r="K60" s="8" t="s">
         <v>139</v>
       </c>
       <c r="L60" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="M60" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N60" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
         <v>94</v>
       </c>
@@ -3896,30 +4078,32 @@
       <c r="D61" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E61" s="11">
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="11">
         <v>5.9118644067796602</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="I61" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H61" s="3"/>
-      <c r="I61" s="5" t="s">
+      <c r="J61" s="3"/>
+      <c r="K61" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="J61" s="32" t="s">
+      <c r="L61" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="K61" s="5">
+      <c r="M61" s="5">
         <v>870</v>
       </c>
-      <c r="L61" s="3" t="s">
+      <c r="N61" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
         <v>94</v>
       </c>
@@ -3932,30 +4116,32 @@
       <c r="D62" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="4">
         <v>9.6406779661016895</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="I62" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H62" s="3"/>
-      <c r="I62" s="5" t="s">
+      <c r="J62" s="3"/>
+      <c r="K62" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="J62" s="32" t="s">
+      <c r="L62" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="K62" s="5">
+      <c r="M62" s="5">
         <v>2158</v>
       </c>
-      <c r="L62" s="3" t="s">
+      <c r="N62" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A63" s="8" t="s">
         <v>94</v>
       </c>
@@ -3968,30 +4154,32 @@
       <c r="D63" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="9">
         <v>40.786440677966098</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="H63" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="I63" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8" t="s">
+      <c r="J63" s="8"/>
+      <c r="K63" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="J63" s="30" t="s">
+      <c r="L63" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="K63" s="8">
+      <c r="M63" s="8">
         <v>1234</v>
       </c>
-      <c r="L63" s="8" t="s">
+      <c r="N63" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
         <v>95</v>
       </c>
@@ -4004,30 +4192,32 @@
       <c r="D64" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E64" s="11">
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="11">
         <v>1.44092219020172</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="H64" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G64" s="11" t="s">
+      <c r="I64" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H64" s="3"/>
-      <c r="I64" s="32" t="s">
+      <c r="J64" s="3"/>
+      <c r="K64" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="J64" s="32" t="s">
+      <c r="L64" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="K64" s="5">
+      <c r="M64" s="5">
         <v>2249</v>
       </c>
-      <c r="L64" s="3" t="s">
+      <c r="N64" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
         <v>95</v>
       </c>
@@ -4040,30 +4230,32 @@
       <c r="D65" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E65" s="11">
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="11">
         <v>4.5533141210374604</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="H65" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="I65" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="32" t="s">
+      <c r="J65" s="3"/>
+      <c r="K65" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="J65" s="32" t="s">
+      <c r="L65" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="K65" s="5">
+      <c r="M65" s="5">
         <v>4785</v>
       </c>
-      <c r="L65" s="3" t="s">
+      <c r="N65" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A66" s="8" t="s">
         <v>95</v>
       </c>
@@ -4076,30 +4268,32 @@
       <c r="D66" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="9">
         <v>83.775216138328503</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="H66" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="I66" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H66" s="8"/>
-      <c r="I66" s="30" t="s">
+      <c r="J66" s="8"/>
+      <c r="K66" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="J66" s="30" t="s">
+      <c r="L66" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="K66" s="8">
+      <c r="M66" s="8">
         <v>805</v>
       </c>
-      <c r="L66" s="8" t="s">
+      <c r="N66" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A67" s="5" t="s">
         <v>96</v>
       </c>
@@ -4112,30 +4306,32 @@
       <c r="D67" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E67" s="11">
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="11">
         <v>1.57232704402515</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="H67" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="I67" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H67" s="3"/>
-      <c r="I67" s="5" t="s">
+      <c r="J67" s="3"/>
+      <c r="K67" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="J67" s="32" t="s">
+      <c r="L67" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K67" s="5">
+      <c r="M67" s="5">
         <v>2601</v>
       </c>
-      <c r="L67" s="5" t="s">
+      <c r="N67" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
         <v>96</v>
       </c>
@@ -4148,30 +4344,32 @@
       <c r="D68" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="4">
         <v>5.3009883198562404</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="H68" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G68" s="4" t="s">
+      <c r="I68" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H68" s="3"/>
-      <c r="I68" s="5" t="s">
+      <c r="J68" s="3"/>
+      <c r="K68" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="J68" s="32" t="s">
+      <c r="L68" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="K68" s="5">
+      <c r="M68" s="5">
         <v>6953</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="N68" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
         <v>96</v>
       </c>
@@ -4184,30 +4382,32 @@
       <c r="D69" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="4">
         <v>4.8966756513926297</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="H69" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="I69" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3" t="s">
+      <c r="J69" s="3"/>
+      <c r="K69" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="J69" s="29" t="s">
+      <c r="L69" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="K69" s="3">
+      <c r="M69" s="3">
         <v>6699</v>
       </c>
-      <c r="L69" s="3" t="s">
+      <c r="N69" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
         <v>96</v>
       </c>
@@ -4220,41 +4420,43 @@
       <c r="D70" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="9">
         <v>0.494159928122192</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="H70" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="I70" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8" t="s">
+      <c r="J70" s="8"/>
+      <c r="K70" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="J70" s="30" t="s">
+      <c r="L70" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="K70" s="8">
+      <c r="M70" s="8">
         <v>1137</v>
       </c>
-      <c r="L70" s="8" t="s">
+      <c r="N70" s="8" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="L58">
+  <conditionalFormatting sqref="N58">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L54">
+  <conditionalFormatting sqref="N54">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="duplicateValues" dxfId="1" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L72:L1048576 C14 C12 C7 L1:L52 L57 L59:L65">
+  <conditionalFormatting sqref="N72:N1048576 C14 C12 C7 N1:N52 N57 N59:N65">
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finish pie hierarchies, start UV mutation analysis
The scripts in 10_Piecharts will not be used for the paper. Instead we will likely quantify UV-associated mutations in cell types along the lines of 11_UV-mut_pDCs
</commit_message>
<xml_diff>
--- a/04_XV-seq/XV-seq_overview.xlsx
+++ b/04_XV-seq/XV-seq_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/scBPDCN-analysis/04_XV-seq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E20708-9821-CC42-8C18-D8C973293D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7AFBFA-DB37-384A-BB87-B94EFF1C95B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="5520" windowWidth="25840" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XV-seq_overview" sheetId="1" r:id="rId1"/>
@@ -1052,7 +1052,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1238,12 +1238,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1423,7 +1417,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1494,12 +1488,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="20" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="22" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1906,8 +1894,8 @@
   <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1986,7 +1974,7 @@
       <c r="D2" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="36" t="s">
         <v>241</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -2028,7 +2016,7 @@
       <c r="D3" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="36" t="s">
         <v>242</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -2070,7 +2058,7 @@
       <c r="D4" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="36" t="s">
         <v>243</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -2114,7 +2102,7 @@
       <c r="D5" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="36" t="s">
         <v>251</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -2158,7 +2146,7 @@
       <c r="D6" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="37" t="s">
         <v>244</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -2202,7 +2190,7 @@
       <c r="D7" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="36" t="s">
         <v>241</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -2244,7 +2232,7 @@
       <c r="D8" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="36" t="s">
         <v>242</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -2286,7 +2274,7 @@
       <c r="D9" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="36" t="s">
         <v>243</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -2330,7 +2318,7 @@
       <c r="D10" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="36" t="s">
         <v>251</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -2374,7 +2362,7 @@
       <c r="D11" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="37" t="s">
         <v>244</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -2418,7 +2406,7 @@
       <c r="D12" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="36" t="s">
         <v>252</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -2460,7 +2448,7 @@
       <c r="D13" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="36" t="s">
         <v>253</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -2502,7 +2490,7 @@
       <c r="D14" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="37" t="s">
         <v>254</v>
       </c>
       <c r="F14" s="9" t="s">
@@ -2544,7 +2532,7 @@
       <c r="D15" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="36" t="s">
         <v>247</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -2588,7 +2576,7 @@
       <c r="D16" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="36" t="s">
         <v>247</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -2632,7 +2620,7 @@
       <c r="D17" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="37" t="s">
         <v>246</v>
       </c>
       <c r="F17" s="9" t="s">
@@ -2676,7 +2664,7 @@
       <c r="D18" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="36" t="s">
         <v>255</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -2720,7 +2708,7 @@
       <c r="D19" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="36" t="s">
         <v>256</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -2764,7 +2752,7 @@
       <c r="D20" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="36" t="s">
         <v>248</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -2805,13 +2793,13 @@
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="4" t="s">
         <v>239</v>
       </c>
       <c r="G21" s="11">
@@ -2852,7 +2840,7 @@
       <c r="D22" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="38" t="s">
         <v>258</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -2896,7 +2884,7 @@
       <c r="D23" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="36" t="s">
         <v>249</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -2937,7 +2925,7 @@
       <c r="D24" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="39" t="s">
         <v>259</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -2981,7 +2969,7 @@
       <c r="D25" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="39" t="s">
         <v>250</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -3022,13 +3010,13 @@
       <c r="C26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="39" t="s">
         <v>260</v>
       </c>
-      <c r="F26" s="38" t="s">
+      <c r="F26" s="11" t="s">
         <v>239</v>
       </c>
       <c r="G26" s="11">
@@ -3066,13 +3054,13 @@
       <c r="C27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="F27" s="38" t="s">
+      <c r="F27" s="11" t="s">
         <v>239</v>
       </c>
       <c r="G27" s="11">
@@ -3113,7 +3101,7 @@
       <c r="D28" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="39" t="s">
         <v>261</v>
       </c>
       <c r="F28" s="11" t="s">
@@ -3245,7 +3233,7 @@
       <c r="D33" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E33" s="45" t="s">
+      <c r="E33" s="39" t="s">
         <v>269</v>
       </c>
       <c r="F33" s="11" t="s">
@@ -3289,7 +3277,7 @@
       <c r="D34" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E34" s="45" t="s">
+      <c r="E34" s="39" t="s">
         <v>262</v>
       </c>
       <c r="F34" s="11" t="s">
@@ -3330,13 +3318,13 @@
       <c r="C35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="E35" s="41" t="s">
+      <c r="D35" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="F35" s="38" t="s">
+      <c r="F35" s="11" t="s">
         <v>239</v>
       </c>
       <c r="G35" s="4">
@@ -3377,7 +3365,7 @@
       <c r="D36" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="37" t="s">
         <v>270</v>
       </c>
       <c r="F36" s="9" t="s">
@@ -3421,10 +3409,10 @@
       <c r="D37" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="F37" s="47" t="s">
+      <c r="F37" s="41" t="s">
         <v>238</v>
       </c>
       <c r="G37" s="4">
@@ -3465,7 +3453,7 @@
       <c r="D38" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="36" t="s">
         <v>256</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -3509,7 +3497,7 @@
       <c r="D39" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="36" t="s">
         <v>248</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -3550,13 +3538,13 @@
       <c r="C40" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E40" s="39" t="s">
+      <c r="E40" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F40" s="4" t="s">
         <v>239</v>
       </c>
       <c r="G40" s="4">
@@ -3597,7 +3585,7 @@
       <c r="D41" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E41" s="48" t="s">
+      <c r="E41" s="42" t="s">
         <v>258</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -3641,7 +3629,7 @@
       <c r="D42" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="36" t="s">
         <v>249</v>
       </c>
       <c r="F42" s="4" t="s">
@@ -3683,7 +3671,7 @@
       <c r="D43" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="36" t="s">
         <v>259</v>
       </c>
       <c r="F43" s="4" t="s">
@@ -3727,7 +3715,7 @@
       <c r="D44" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E44" s="36" t="s">
         <v>250</v>
       </c>
       <c r="F44" s="4" t="s">
@@ -3768,13 +3756,13 @@
       <c r="C45" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D45" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E45" s="39" t="s">
+      <c r="E45" s="36" t="s">
         <v>260</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="4" t="s">
         <v>239</v>
       </c>
       <c r="G45" s="4">
@@ -3812,13 +3800,13 @@
       <c r="C46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E46" s="39" t="s">
+      <c r="E46" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="4" t="s">
         <v>239</v>
       </c>
       <c r="G46" s="4">
@@ -3859,7 +3847,7 @@
       <c r="D47" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E47" s="42" t="s">
+      <c r="E47" s="36" t="s">
         <v>261</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -3991,7 +3979,7 @@
       <c r="D52" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E52" s="43" t="s">
+      <c r="E52" s="37" t="s">
         <v>269</v>
       </c>
       <c r="F52" s="9" t="s">
@@ -4035,7 +4023,7 @@
       <c r="D53" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E53" s="42" t="s">
+      <c r="E53" s="36" t="s">
         <v>264</v>
       </c>
       <c r="F53" s="4" t="s">
@@ -4074,13 +4062,13 @@
       <c r="C54" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E54" s="39" t="s">
+      <c r="E54" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="F54" s="36" t="s">
+      <c r="F54" s="4" t="s">
         <v>239</v>
       </c>
       <c r="G54" s="4">
@@ -4121,7 +4109,7 @@
       <c r="D55" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="36" t="s">
         <v>272</v>
       </c>
       <c r="F55" s="4" t="s">
@@ -4165,7 +4153,7 @@
       <c r="D56" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="37" t="s">
         <v>273</v>
       </c>
       <c r="F56" s="9" t="s">
@@ -4209,7 +4197,7 @@
       <c r="D57" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E57" s="42" t="s">
+      <c r="E57" s="36" t="s">
         <v>264</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -4248,13 +4236,13 @@
       <c r="C58" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D58" s="36" t="s">
+      <c r="D58" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E58" s="39" t="s">
+      <c r="E58" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="F58" s="36" t="s">
+      <c r="F58" s="4" t="s">
         <v>239</v>
       </c>
       <c r="G58" s="4">
@@ -4295,7 +4283,7 @@
       <c r="D59" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E59" s="42" t="s">
+      <c r="E59" s="36" t="s">
         <v>272</v>
       </c>
       <c r="F59" s="4" t="s">
@@ -4339,7 +4327,7 @@
       <c r="D60" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="E60" s="37" t="s">
         <v>273</v>
       </c>
       <c r="F60" s="9" t="s">
@@ -4383,10 +4371,10 @@
       <c r="D61" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E61" s="41" t="s">
+      <c r="E61" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="F61" s="38" t="s">
+      <c r="F61" s="11" t="s">
         <v>239</v>
       </c>
       <c r="G61" s="11">
@@ -4427,7 +4415,7 @@
       <c r="D62" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E62" s="42" t="s">
+      <c r="E62" s="36" t="s">
         <v>274</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -4469,7 +4457,7 @@
       <c r="D63" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E63" s="43" t="s">
+      <c r="E63" s="37" t="s">
         <v>275</v>
       </c>
       <c r="F63" s="9" t="s">
@@ -4511,7 +4499,7 @@
       <c r="D64" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="45" t="s">
+      <c r="E64" s="39" t="s">
         <v>276</v>
       </c>
       <c r="F64" s="11" t="s">
@@ -4553,7 +4541,7 @@
       <c r="D65" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E65" s="45" t="s">
+      <c r="E65" s="39" t="s">
         <v>277</v>
       </c>
       <c r="F65" s="11" t="s">
@@ -4595,10 +4583,10 @@
       <c r="D66" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E66" s="40" t="s">
+      <c r="E66" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="F66" s="37" t="s">
+      <c r="F66" s="9" t="s">
         <v>239</v>
       </c>
       <c r="G66" s="9">
@@ -4637,7 +4625,7 @@
       <c r="D67" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E67" s="45" t="s">
+      <c r="E67" s="39" t="s">
         <v>266</v>
       </c>
       <c r="F67" s="11" t="s">
@@ -4679,7 +4667,7 @@
       <c r="D68" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E68" s="42" t="s">
+      <c r="E68" s="36" t="s">
         <v>279</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -4721,7 +4709,7 @@
       <c r="D69" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E69" s="42" t="s">
+      <c r="E69" s="36" t="s">
         <v>241</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -4763,7 +4751,7 @@
       <c r="D70" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E70" s="43" t="s">
+      <c r="E70" s="37" t="s">
         <v>267</v>
       </c>
       <c r="F70" s="9" t="s">

</xml_diff>